<commit_message>
Ahhhh, le Bikini Bottom
</commit_message>
<xml_diff>
--- a/Clark_Joel_Week3_Risk_Register.xlsx
+++ b/Clark_Joel_Week3_Risk_Register.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/05083b2baa634b45/School/Spring 2022/Real-Time Operating Systems/Final Project/final-project-week4-thejclark96/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="14_{32CEC08C-A6AD-4531-BC99-5EDDD1F8FE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{640B3BA5-52C7-43DA-BAEC-B6FB816ACCD4}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="14_{32CEC08C-A6AD-4531-BC99-5EDDD1F8FE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0F00997-B088-45A3-8E68-CA123F706538}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18180" yWindow="990" windowWidth="18360" windowHeight="29160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1550,7 +1550,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>